<commit_message>
Got some work done for the charcter model
</commit_message>
<xml_diff>
--- a/Scedule_Hite.xlsx
+++ b/Scedule_Hite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Spring2018_ProjectPlus\Spring2018_ProjectPlus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD59831-4451-4F9D-824D-06300820AD22}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A116033-E75F-44E6-95E2-3DCB25B5EC96}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,8 +385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +583,7 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K6" s="1">
         <v>43170</v>
@@ -669,6 +669,18 @@
       <c r="A9" s="1">
         <v>43173</v>
       </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
       <c r="K9" s="1">
         <v>43173</v>
       </c>
@@ -748,23 +760,23 @@
     <row r="13" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="3">
         <f>SUM(C6:C12)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="3">
         <f>SUM(D6:D12)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E13" s="3">
         <f>SUM(E6:E12)</f>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="F13" s="3">
         <f>SUM(F6:F12)</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G13" s="3">
         <f>SUM(C13:F13)</f>
-        <v>23.5</v>
+        <v>32.5</v>
       </c>
       <c r="M13" s="3">
         <f>SUM(M6:M12)</f>
@@ -1167,7 +1179,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4">
         <f>SUM(G21,G13,G5)</f>
-        <v>44.5</v>
+        <v>53.5</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -2149,7 +2161,7 @@
       <c r="F76" s="5"/>
       <c r="G76" s="5">
         <f>SUM(G74,G64,G56,G48,G40,G21,G13,G5)</f>
-        <v>44.5</v>
+        <v>53.5</v>
       </c>
       <c r="K76" s="1"/>
       <c r="M76" s="5"/>

</xml_diff>